<commit_message>
Removed unncessary entity objects like: activity, article, topic, quiz
</commit_message>
<xml_diff>
--- a/scripts/maui_topics.xlsx
+++ b/scripts/maui_topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/dev/chimple/maui/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4122A1-AA65-5E49-93F7-DF3A6F0F9761}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1D0D89-DBEA-5546-B30C-21A703254B90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="460" windowWidth="22900" windowHeight="16160" xr2:uid="{923C0303-3085-0A4F-97FA-EF093955F0A8}"/>
   </bookViews>
@@ -1041,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4347587-5860-5840-846F-B3CE617B1DE6}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Refactored into quack package to accomodate new look
</commit_message>
<xml_diff>
--- a/scripts/maui_topics.xlsx
+++ b/scripts/maui_topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/dev/chimple/maui/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1D0D89-DBEA-5546-B30C-21A703254B90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E69D65D-F1BE-8845-BAFA-909D0F78DCDC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="460" windowWidth="22900" windowHeight="16160" xr2:uid="{923C0303-3085-0A4F-97FA-EF093955F0A8}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="181">
   <si>
     <t>topic</t>
   </si>
@@ -655,6 +655,9 @@
   </si>
   <si>
     <t>Draw a picture of a tiger and add a roar on it</t>
+  </si>
+  <si>
+    <t>Main</t>
   </si>
 </sst>
 </file>
@@ -1039,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4347587-5860-5840-846F-B3CE617B1DE6}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1387,272 +1390,302 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>87</v>
+        <v>144</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1660,16 +1693,16 @@
         <v>125</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -1677,31 +1710,31 @@
         <v>144</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -1709,32 +1742,32 @@
         <v>176</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -1742,7 +1775,7 @@
         <v>144</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -1750,7 +1783,7 @@
         <v>144</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -1758,7 +1791,7 @@
         <v>144</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -1766,24 +1799,15 @@
         <v>144</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -1791,177 +1815,442 @@
         <v>144</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>178</v>
+        <v>95</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>